<commit_message>
docs: ajout d'avertissement étudiant et suppression mentions confidentielles
</commit_message>
<xml_diff>
--- a/exemples_excel_access/output/donnees_erp.xlsx
+++ b/exemples_excel_access/output/donnees_erp.xlsx
@@ -469,7 +469,7 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2026-02-17 18:13</t>
+          <t>2026-02-18 09:29</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -490,7 +490,7 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2026-02-17 19:13</t>
+          <t>2026-02-18 10:29</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -511,7 +511,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2026-02-17 20:13</t>
+          <t>2026-02-18 11:29</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -532,7 +532,7 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2026-02-17 21:13</t>
+          <t>2026-02-18 12:29</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -553,7 +553,7 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2026-02-17 22:13</t>
+          <t>2026-02-18 13:29</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -574,7 +574,7 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2026-02-17 23:13</t>
+          <t>2026-02-18 14:29</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -595,7 +595,7 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2026-02-18 00:13</t>
+          <t>2026-02-18 15:29</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -616,7 +616,7 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2026-02-18 01:13</t>
+          <t>2026-02-18 16:29</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -637,7 +637,7 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2026-02-18 02:13</t>
+          <t>2026-02-18 17:29</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -658,7 +658,7 @@
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2026-02-18 03:13</t>
+          <t>2026-02-18 18:29</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -679,7 +679,7 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2026-02-18 04:13</t>
+          <t>2026-02-18 19:29</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -700,7 +700,7 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2026-02-18 05:13</t>
+          <t>2026-02-18 20:29</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -721,7 +721,7 @@
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2026-02-18 06:13</t>
+          <t>2026-02-18 21:29</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -742,7 +742,7 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2026-02-18 07:13</t>
+          <t>2026-02-18 22:29</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -763,7 +763,7 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2026-02-18 08:13</t>
+          <t>2026-02-18 23:29</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -784,7 +784,7 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2026-02-18 09:13</t>
+          <t>2026-02-19 00:29</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -805,7 +805,7 @@
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2026-02-18 10:13</t>
+          <t>2026-02-19 01:29</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -826,7 +826,7 @@
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2026-02-18 11:13</t>
+          <t>2026-02-19 02:29</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -847,7 +847,7 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2026-02-18 12:13</t>
+          <t>2026-02-19 03:29</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -868,7 +868,7 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2026-02-18 13:13</t>
+          <t>2026-02-19 04:29</t>
         </is>
       </c>
       <c r="D21" t="n">

</xml_diff>